<commit_message>
CHF Market: removed broken link 4.30.2015
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/CHF/CHF_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/CHF/CHF_MainChecks.xlsx
@@ -814,28 +814,28 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 17:05:37</v>
+        <v>Updated at 16:02:55</v>
         <stp/>
-        <stp>{1BC20190-FE7A-481E-A49A-44D708D13EC2}</stp>
-        <tr r="P7" s="2"/>
+        <stp>{0B739ED6-7596-4829-BEED-9F27B171E83E}</stp>
+        <tr r="Q7" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 17:04:50</v>
+        <v>Updated at 16:04:31</v>
         <stp/>
-        <stp>{FE2F3133-59D8-47B5-86BD-66B0AE42C501}</stp>
+        <stp>{859AE018-88F3-47E5-AF4B-DCE96851888B}</stp>
         <tr r="Q6" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 17:06:43</v>
+        <v>Updated at 16:04:39</v>
         <stp/>
-        <stp>{706D2534-F369-44E4-8F58-F34BADECA9E3}</stp>
+        <stp>{FEA7DC95-2BD7-4569-95E6-204C9917FA19}</stp>
         <tr r="Q5" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 17:05:37</v>
+        <v>Updated at 16:02:55</v>
         <stp/>
-        <stp>{4B24D794-C1CA-4255-A4C3-EBB536736645}</stp>
-        <tr r="Q7" s="2"/>
+        <stp>{AB59C335-2F81-4495-AC61-3E0494760040}</stp>
+        <tr r="P7" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1322,9 +1322,7 @@
       <c r="T2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="18">
-        <v>42118.650057870371</v>
-      </c>
+      <c r="U2" s="18"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -1486,14 +1484,14 @@
         <v>42163</v>
       </c>
       <c r="M5" s="28">
-        <v>159.30000000000001</v>
+        <v>156.83000000000001</v>
       </c>
       <c r="N5" s="28"/>
       <c r="O5" s="28"/>
       <c r="P5" s="28"/>
       <c r="Q5" s="29" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 17:06:43</v>
+        <v>Updated at 16:04:39</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>11</v>
@@ -1556,14 +1554,14 @@
         <v>42170</v>
       </c>
       <c r="M6" s="59">
-        <v>100.88</v>
+        <v>100.82000000000001</v>
       </c>
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
       <c r="Q6" s="31" t="str">
         <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>Updated at 17:04:50</v>
+        <v>Updated at 16:04:31</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>11</v>
@@ -1574,7 +1572,7 @@
       </c>
       <c r="U6" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>492</v>
+        <v>745</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1624,25 +1622,25 @@
         <v>CHFAB3L10Y</v>
       </c>
       <c r="L7" s="24">
-        <v>42118</v>
+        <v>42124</v>
       </c>
       <c r="M7" s="33" t="str">
         <f>N7&amp;"/"&amp;O7</f>
-        <v>-0.0425/0.0375</v>
+        <v>0.0775/0.1575</v>
       </c>
       <c r="N7" s="30">
-        <v>-4.2500000000000003E-2</v>
+        <v>7.7499999999999999E-2</v>
       </c>
       <c r="O7" s="30">
-        <v>3.7499999999999999E-2</v>
+        <v>0.1575</v>
       </c>
       <c r="P7" s="30" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Updated at 17:05:37</v>
+        <v>Updated at 16:02:55</v>
       </c>
       <c r="Q7" s="31" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Updated at 17:05:37</v>
+        <v>Updated at 16:02:55</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>11</v>
@@ -1823,11 +1821,11 @@
       </c>
       <c r="L10" s="22">
         <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>42109</v>
+        <v>42124</v>
       </c>
       <c r="M10" s="32">
         <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>-8.1200000000000005E-3</v>
+        <v>-7.9400000000000009E-3</v>
       </c>
       <c r="N10" s="32"/>
       <c r="O10" s="32"/>
@@ -1901,7 +1899,7 @@
       <c r="P11" s="25"/>
       <c r="Q11" s="35" t="str">
         <f ca="1">IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <v/>
       </c>
       <c r="R11" s="8" t="s">
         <v>11</v>
@@ -1956,9 +1954,9 @@
         <f>UPPER(Currency)&amp;"ON"</f>
         <v>CHFON</v>
       </c>
-      <c r="L12" s="24" t="e">
+      <c r="L12" s="24">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>#NUM!</v>
+        <v>42124</v>
       </c>
       <c r="M12" s="25">
         <v>0</v>
@@ -1967,8 +1965,8 @@
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
       <c r="Q12" s="35" t="str">
-        <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
+        <v/>
       </c>
       <c r="R12" s="8" t="s">
         <v>11</v>
@@ -2035,7 +2033,7 @@
       <c r="P13" s="25"/>
       <c r="Q13" s="36" t="str">
         <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <v/>
       </c>
       <c r="R13" s="8" t="s">
         <v>11</v>
@@ -2086,7 +2084,7 @@
       <c r="P14" s="25"/>
       <c r="Q14" s="36" t="str">
         <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <v/>
       </c>
       <c r="R14" s="8" t="s">
         <v>11</v>
@@ -2145,7 +2143,7 @@
       <c r="P15" s="25"/>
       <c r="Q15" s="36" t="str">
         <f ca="1">IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <v/>
       </c>
       <c r="R15" s="8" t="s">
         <v>11</v>
@@ -2202,7 +2200,7 @@
       <c r="P16" s="44"/>
       <c r="Q16" s="45" t="str">
         <f ca="1">IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
-        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID 'CHF1Y'</v>
+        <v/>
       </c>
       <c r="R16" s="8" t="s">
         <v>11</v>
@@ -5481,7 +5479,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="CommandButton1">
+        <control shapeId="1026" r:id="rId4" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5501,12 +5499,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="CommandButton2">
+        <control shapeId="1025" r:id="rId6" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5526,7 +5524,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
CHF Market: review curves 05.05.2015
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/CHF/CHF_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/CHF/CHF_MainChecks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9585" yWindow="-15" windowWidth="9630" windowHeight="12015"/>
+    <workbookView xWindow="-15" yWindow="7965" windowWidth="19230" windowHeight="4035"/>
   </bookViews>
   <sheets>
     <sheet name="MainChecks" sheetId="2" r:id="rId1"/>
@@ -813,28 +813,28 @@
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
-      <tp t="s">
-        <v>Updated at 16:02:55</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
-        <stp>{0B739ED6-7596-4829-BEED-9F27B171E83E}</stp>
+        <stp>{EDE25FC2-601A-428D-96D6-385C4DCEB2A2}</stp>
+        <tr r="Q5" s="2"/>
+      </tp>
+      <tp t="e">
+        <v>#N/A</v>
+        <stp/>
+        <stp>{42FEB5B3-0553-4E7A-B22E-CEC26BEA9A45}</stp>
+        <tr r="Q6" s="2"/>
+      </tp>
+      <tp t="e">
+        <v>#N/A</v>
+        <stp/>
+        <stp>{99CC1CA7-9AB2-4EA1-B03E-7140743B01A7}</stp>
         <tr r="Q7" s="2"/>
       </tp>
-      <tp t="s">
-        <v>Updated at 16:04:31</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
-        <stp>{859AE018-88F3-47E5-AF4B-DCE96851888B}</stp>
-        <tr r="Q6" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 16:04:39</v>
-        <stp/>
-        <stp>{FEA7DC95-2BD7-4569-95E6-204C9917FA19}</stp>
-        <tr r="Q5" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 16:02:55</v>
-        <stp/>
-        <stp>{AB59C335-2F81-4495-AC61-3E0494760040}</stp>
+        <stp>{D6D1B3A5-3241-44AD-9BB1-3FC18F62E497}</stp>
         <tr r="P7" s="2"/>
       </tp>
     </main>
@@ -1322,7 +1322,9 @@
       <c r="T2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="18"/>
+      <c r="U2" s="18">
+        <v>42129.662268518521</v>
+      </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -1489,9 +1491,9 @@
       <c r="N5" s="28"/>
       <c r="O5" s="28"/>
       <c r="P5" s="28"/>
-      <c r="Q5" s="29" t="str">
+      <c r="Q5" s="29">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 16:04:39</v>
+        <v>0</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>11</v>
@@ -1559,9 +1561,9 @@
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
-      <c r="Q6" s="31" t="str">
+      <c r="Q6" s="31">
         <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>Updated at 16:04:31</v>
+        <v>0</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>11</v>
@@ -1572,7 +1574,7 @@
       </c>
       <c r="U6" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>745</v>
+        <v>1016</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1634,13 +1636,13 @@
       <c r="O7" s="30">
         <v>0.1575</v>
       </c>
-      <c r="P7" s="30" t="str">
+      <c r="P7" s="30">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Updated at 16:02:55</v>
-      </c>
-      <c r="Q7" s="31" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="31">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Updated at 16:02:55</v>
+        <v>0</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>11</v>
@@ -1821,11 +1823,11 @@
       </c>
       <c r="L10" s="22">
         <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>42124</v>
+        <v>42125</v>
       </c>
       <c r="M10" s="32">
         <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>-7.9400000000000009E-3</v>
+        <v>-7.9500000000000005E-3</v>
       </c>
       <c r="N10" s="32"/>
       <c r="O10" s="32"/>
@@ -1887,9 +1889,9 @@
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>CHFSTD</v>
       </c>
-      <c r="L11" s="24" t="e">
+      <c r="L11" s="24">
         <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>#NUM!</v>
+        <v>42129</v>
       </c>
       <c r="M11" s="25">
         <v>0</v>
@@ -1898,7 +1900,7 @@
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
       <c r="Q11" s="35" t="str">
-        <f ca="1">IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
+        <f>IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
         <v/>
       </c>
       <c r="R11" s="8" t="s">
@@ -1956,7 +1958,7 @@
       </c>
       <c r="L12" s="24">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>42124</v>
+        <v>42129</v>
       </c>
       <c r="M12" s="25">
         <v>0</v>
@@ -2021,9 +2023,9 @@
         <f>UPPER(Currency)&amp;"1M"</f>
         <v>CHF1M</v>
       </c>
-      <c r="L13" s="24" t="e">
+      <c r="L13" s="24">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>#NUM!</v>
+        <v>42131</v>
       </c>
       <c r="M13" s="25">
         <v>0</v>
@@ -2032,7 +2034,7 @@
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
       <c r="Q13" s="36" t="str">
-        <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
+        <f>IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
         <v/>
       </c>
       <c r="R13" s="8" t="s">
@@ -2072,9 +2074,9 @@
         <f>UPPER(Currency)&amp;"3M"</f>
         <v>CHF3M</v>
       </c>
-      <c r="L14" s="24" t="e">
+      <c r="L14" s="24">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>#NUM!</v>
+        <v>42131</v>
       </c>
       <c r="M14" s="25">
         <v>0</v>
@@ -2083,7 +2085,7 @@
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
       <c r="Q14" s="36" t="str">
-        <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
+        <f>IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
         <v/>
       </c>
       <c r="R14" s="8" t="s">
@@ -2131,9 +2133,9 @@
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>CHF6M</v>
       </c>
-      <c r="L15" s="24" t="e">
+      <c r="L15" s="24">
         <f>_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
-        <v>#NUM!</v>
+        <v>42131</v>
       </c>
       <c r="M15" s="25">
         <v>0</v>
@@ -2142,7 +2144,7 @@
       <c r="O15" s="25"/>
       <c r="P15" s="25"/>
       <c r="Q15" s="36" t="str">
-        <f ca="1">IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
+        <f>IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
         <v/>
       </c>
       <c r="R15" s="8" t="s">
@@ -2200,7 +2202,7 @@
       <c r="P16" s="44"/>
       <c r="Q16" s="45" t="str">
         <f ca="1">IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
-        <v/>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID 'CHF1Y'</v>
       </c>
       <c r="R16" s="8" t="s">
         <v>11</v>
@@ -5479,7 +5481,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CommandButton2">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5499,12 +5501,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="CommandButton1">
+        <control shapeId="1026" r:id="rId6" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5524,7 +5526,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
CHF Model: modified monitor curves 06.05.2015
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/CHF/CHF_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/CHF/CHF_MainChecks.xlsx
@@ -586,7 +586,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -718,6 +718,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="1"/>
@@ -813,29 +816,29 @@
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
-      <tp t="e">
-        <v>#N/A</v>
+      <tp t="s">
+        <v>Updated at 08:06:32</v>
         <stp/>
-        <stp>{EDE25FC2-601A-428D-96D6-385C4DCEB2A2}</stp>
+        <stp>{87AD9020-5A74-4216-A7FC-0D50C5E0DB7E}</stp>
         <tr r="Q5" s="2"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+      <tp t="s">
+        <v>Updated at 08:03:08</v>
         <stp/>
-        <stp>{42FEB5B3-0553-4E7A-B22E-CEC26BEA9A45}</stp>
-        <tr r="Q6" s="2"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>{99CC1CA7-9AB2-4EA1-B03E-7140743B01A7}</stp>
+        <stp>{C6AAD86A-B589-44C7-B211-943D11BEFD9A}</stp>
         <tr r="Q7" s="2"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+      <tp t="s">
+        <v>Updated at 08:03:08</v>
         <stp/>
-        <stp>{D6D1B3A5-3241-44AD-9BB1-3FC18F62E497}</stp>
+        <stp>{6CF2910D-8C59-4F77-831E-30A8B06950BF}</stp>
         <tr r="P7" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 08:03:08</v>
+        <stp/>
+        <stp>{C998CAFB-D698-4FFE-948E-24C12C5E740E}</stp>
+        <tr r="Q6" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1323,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="U2" s="18">
-        <v>42129.662268518521</v>
+        <v>42130.335358796299</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
@@ -1486,14 +1489,14 @@
         <v>42163</v>
       </c>
       <c r="M5" s="28">
-        <v>156.83000000000001</v>
+        <v>154.74</v>
       </c>
       <c r="N5" s="28"/>
       <c r="O5" s="28"/>
       <c r="P5" s="28"/>
-      <c r="Q5" s="29">
+      <c r="Q5" s="29" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>0</v>
+        <v>Updated at 08:06:32</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>11</v>
@@ -1556,14 +1559,14 @@
         <v>42170</v>
       </c>
       <c r="M6" s="59">
-        <v>100.82000000000001</v>
+        <v>0</v>
       </c>
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
-      <c r="Q6" s="31">
+      <c r="Q6" s="31" t="str">
         <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>0</v>
+        <v>Updated at 08:03:08</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>11</v>
@@ -1574,7 +1577,7 @@
       </c>
       <c r="U6" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>1016</v>
+        <v>1044</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1624,25 +1627,25 @@
         <v>CHFAB3L10Y</v>
       </c>
       <c r="L7" s="24">
-        <v>42124</v>
+        <v>42129</v>
       </c>
       <c r="M7" s="33" t="str">
         <f>N7&amp;"/"&amp;O7</f>
-        <v>0.0775/0.1575</v>
+        <v>0.16/0.24</v>
       </c>
       <c r="N7" s="30">
-        <v>7.7499999999999999E-2</v>
+        <v>0.16</v>
       </c>
       <c r="O7" s="30">
-        <v>0.1575</v>
-      </c>
-      <c r="P7" s="30">
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="P7" s="30" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="31">
+        <v>Updated at 08:03:08</v>
+      </c>
+      <c r="Q7" s="31" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>0</v>
+        <v>Updated at 08:03:08</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>11</v>
@@ -1891,7 +1894,7 @@
       </c>
       <c r="L11" s="24">
         <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>42129</v>
+        <v>42130</v>
       </c>
       <c r="M11" s="25">
         <v>0</v>
@@ -1958,7 +1961,7 @@
       </c>
       <c r="L12" s="24">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>42129</v>
+        <v>42130</v>
       </c>
       <c r="M12" s="25">
         <v>0</v>
@@ -2025,7 +2028,7 @@
       </c>
       <c r="L13" s="24">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>42131</v>
+        <v>42132</v>
       </c>
       <c r="M13" s="25">
         <v>0</v>
@@ -2076,7 +2079,7 @@
       </c>
       <c r="L14" s="24">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>42131</v>
+        <v>42132</v>
       </c>
       <c r="M14" s="25">
         <v>0</v>
@@ -2129,21 +2132,21 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="23" t="str">
+      <c r="K15" s="43" t="str">
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>CHF6M</v>
       </c>
-      <c r="L15" s="24">
+      <c r="L15" s="61">
         <f>_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
-        <v>42131</v>
-      </c>
-      <c r="M15" s="25">
+        <v>42132</v>
+      </c>
+      <c r="M15" s="44">
         <v>0</v>
       </c>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="36" t="str">
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
+      <c r="Q15" s="45" t="str">
         <f>IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
         <v/>
       </c>
@@ -2169,7 +2172,7 @@
       <c r="AI15" s="3"/>
       <c r="AJ15" s="3"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="40" t="b">
         <v>1</v>
@@ -2185,26 +2188,18 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="43" t="str">
-        <f>UPPER(Currency)&amp;"1Y"</f>
-        <v>CHF1Y</v>
-      </c>
-      <c r="L16" s="24" t="e">
-        <f>_xll.qlTermStructureReferenceDate(K16,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M16" s="44">
-        <v>0</v>
-      </c>
-      <c r="N16" s="44"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
-      <c r="Q16" s="45" t="str">
-        <f ca="1">IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
-        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID 'CHF1Y'</v>
-      </c>
-      <c r="R16" s="8" t="s">
+      <c r="J16" s="9"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="42" t="str">
+        <f>IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
+        <v/>
+      </c>
+      <c r="R16" s="10" t="s">
         <v>11</v>
       </c>
       <c r="S16" s="1"/>
@@ -2226,7 +2221,7 @@
       <c r="AI16" s="3"/>
       <c r="AJ16" s="3"/>
     </row>
-    <row r="17" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="40" t="b">
         <v>1</v>
@@ -2242,15 +2237,15 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="10" t="s">
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="S17" s="1"/>
@@ -2290,13 +2285,13 @@
       <c r="I18" s="3"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="L18" s="3"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
+      <c r="O18" s="3"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
+      <c r="R18" s="3"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
@@ -2328,13 +2323,13 @@
       <c r="I19" s="3"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="L19" s="3"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="O19" s="3"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
+      <c r="R19" s="3"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -2366,13 +2361,13 @@
       <c r="I20" s="3"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="L20" s="3"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
+      <c r="O20" s="3"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+      <c r="R20" s="3"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
@@ -2404,13 +2399,13 @@
       <c r="I21" s="3"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="L21" s="3"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+      <c r="O21" s="3"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+      <c r="R21" s="3"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
@@ -2442,13 +2437,13 @@
       <c r="I22" s="3"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="L22" s="3"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
+      <c r="O22" s="3"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
+      <c r="R22" s="3"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -5481,7 +5476,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="CommandButton1">
+        <control shapeId="1026" r:id="rId4" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5501,12 +5496,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="CommandButton2">
+        <control shapeId="1025" r:id="rId6" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5526,7 +5521,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
CHF Market: final review 05.08.2015
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/CHF/CHF_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/CHF/CHF_MainChecks.xlsx
@@ -817,27 +817,27 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 08:06:32</v>
+        <v>Updated at 08:58:21</v>
         <stp/>
-        <stp>{87AD9020-5A74-4216-A7FC-0D50C5E0DB7E}</stp>
+        <stp>{45F429B7-C75C-4F74-B167-C6CBC7B85B99}</stp>
+        <tr r="P7" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 08:39:36</v>
+        <stp/>
+        <stp>{7D3649D3-23CF-499C-95BE-CDACC837D956}</stp>
+        <tr r="Q7" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 08:59:57</v>
+        <stp/>
+        <stp>{451A19DD-1566-45CC-8EC6-DC80F55ED189}</stp>
         <tr r="Q5" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 08:03:08</v>
+        <v>Updated at 08:39:36</v>
         <stp/>
-        <stp>{C6AAD86A-B589-44C7-B211-943D11BEFD9A}</stp>
-        <tr r="Q7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 08:03:08</v>
-        <stp/>
-        <stp>{6CF2910D-8C59-4F77-831E-30A8B06950BF}</stp>
-        <tr r="P7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 08:03:08</v>
-        <stp/>
-        <stp>{C998CAFB-D698-4FFE-948E-24C12C5E740E}</stp>
+        <stp>{30A9EB97-CC91-4113-A1B7-DBBC4721B64F}</stp>
         <tr r="Q6" s="2"/>
       </tp>
     </main>
@@ -1325,9 +1325,7 @@
       <c r="T2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="18">
-        <v>42130.335358796299</v>
-      </c>
+      <c r="U2" s="18"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -1489,14 +1487,14 @@
         <v>42163</v>
       </c>
       <c r="M5" s="28">
-        <v>154.74</v>
+        <v>154.77000000000001</v>
       </c>
       <c r="N5" s="28"/>
       <c r="O5" s="28"/>
       <c r="P5" s="28"/>
       <c r="Q5" s="29" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 08:06:32</v>
+        <v>Updated at 08:59:57</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>11</v>
@@ -1559,14 +1557,14 @@
         <v>42170</v>
       </c>
       <c r="M6" s="59">
-        <v>0</v>
+        <v>100.82000000000001</v>
       </c>
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
       <c r="Q6" s="31" t="str">
         <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>Updated at 08:03:08</v>
+        <v>Updated at 08:39:36</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>11</v>
@@ -1577,7 +1575,7 @@
       </c>
       <c r="U6" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>1044</v>
+        <v>1094</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1627,25 +1625,25 @@
         <v>CHFAB3L10Y</v>
       </c>
       <c r="L7" s="24">
-        <v>42129</v>
+        <v>42132</v>
       </c>
       <c r="M7" s="33" t="str">
         <f>N7&amp;"/"&amp;O7</f>
-        <v>0.16/0.24</v>
+        <v>0.1825/0.2625</v>
       </c>
       <c r="N7" s="30">
-        <v>0.16</v>
+        <v>0.1825</v>
       </c>
       <c r="O7" s="30">
-        <v>0.24000000000000002</v>
+        <v>0.26250000000000001</v>
       </c>
       <c r="P7" s="30" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Updated at 08:03:08</v>
+        <v>Updated at 08:58:21</v>
       </c>
       <c r="Q7" s="31" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Updated at 08:03:08</v>
+        <v>Updated at 08:39:36</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>11</v>
@@ -1826,11 +1824,11 @@
       </c>
       <c r="L10" s="22">
         <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>42125</v>
+        <v>42131</v>
       </c>
       <c r="M10" s="32">
         <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>-7.9500000000000005E-3</v>
+        <v>-7.92E-3</v>
       </c>
       <c r="N10" s="32"/>
       <c r="O10" s="32"/>
@@ -1894,10 +1892,11 @@
       </c>
       <c r="L11" s="24">
         <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>42130</v>
+        <v>42132</v>
       </c>
       <c r="M11" s="25">
-        <v>0</v>
+        <f>_xll.qlYieldTSDiscount(K11,L11)</f>
+        <v>1</v>
       </c>
       <c r="N11" s="25"/>
       <c r="O11" s="25"/>
@@ -1961,10 +1960,11 @@
       </c>
       <c r="L12" s="24">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>42130</v>
+        <v>42135</v>
       </c>
       <c r="M12" s="25">
-        <v>0</v>
+        <f>_xll.qlYieldTSDiscount(K12,L12)</f>
+        <v>1</v>
       </c>
       <c r="N12" s="25"/>
       <c r="O12" s="25"/>
@@ -2028,10 +2028,11 @@
       </c>
       <c r="L13" s="24">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>42132</v>
+        <v>42136</v>
       </c>
       <c r="M13" s="25">
-        <v>0</v>
+        <f>_xll.qlYieldTSDiscount(K13,L13)</f>
+        <v>1</v>
       </c>
       <c r="N13" s="25"/>
       <c r="O13" s="25"/>
@@ -2079,10 +2080,11 @@
       </c>
       <c r="L14" s="24">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>42132</v>
+        <v>42136</v>
       </c>
       <c r="M14" s="25">
-        <v>0</v>
+        <f>_xll.qlYieldTSDiscount(K14,L14)</f>
+        <v>1</v>
       </c>
       <c r="N14" s="25"/>
       <c r="O14" s="25"/>
@@ -2138,10 +2140,11 @@
       </c>
       <c r="L15" s="61">
         <f>_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
-        <v>42132</v>
+        <v>42136</v>
       </c>
       <c r="M15" s="44">
-        <v>0</v>
+        <f>_xll.qlYieldTSDiscount(K15,L15)</f>
+        <v>1</v>
       </c>
       <c r="N15" s="44"/>
       <c r="O15" s="44"/>

</xml_diff>